<commit_message>
excel_writer: also include totals for the balance columns
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_write_results_all.xlsx
+++ b/tests/expected_results/result_test_write_results_all.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3052" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3050" uniqueCount="31">
   <si>
     <t xml:space="preserve">Plattform</t>
   </si>
@@ -31542,7 +31542,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31985,11 +31985,11 @@
         <v>30</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
+      <c r="C12" s="2" t="n">
+        <v>1265.29</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>91.29</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>-54263.16</v>

</xml_diff>